<commit_message>
Implemented Year 2 Dashboard for MacOS
</commit_message>
<xml_diff>
--- a/Data/parkInformationGeodesic.xlsx
+++ b/Data/parkInformationGeodesic.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/austinlackey/Documents/GitHub/nps-sem/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89DA5F05-C940-8F47-BD00-82EB20DC4439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F28CAB2-B8ED-F04C-8680-4A4E68279A1D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26020" windowHeight="31500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="43620" windowHeight="31500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6346" uniqueCount="2230">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6321" uniqueCount="2230">
   <si>
     <t>park_id</t>
   </si>
@@ -7075,11 +7075,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T407"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
-      <selection activeCell="S174" sqref="S174"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="M30" sqref="M30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="11" max="11" width="23.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
@@ -7163,7 +7166,7 @@
         <v>24</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H2" t="s">
         <v>25</v>
@@ -7219,7 +7222,7 @@
         <v>36</v>
       </c>
       <c r="G3">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H3" t="s">
         <v>25</v>
@@ -7275,7 +7278,7 @@
         <v>47</v>
       </c>
       <c r="G4">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H4" t="s">
         <v>25</v>
@@ -7331,7 +7334,7 @@
         <v>57</v>
       </c>
       <c r="G5">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H5" t="s">
         <v>25</v>
@@ -7387,7 +7390,7 @@
         <v>66</v>
       </c>
       <c r="G6">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H6" t="s">
         <v>25</v>
@@ -7443,7 +7446,7 @@
         <v>77</v>
       </c>
       <c r="G7">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H7" t="s">
         <v>78</v>
@@ -7505,7 +7508,7 @@
         <v>36</v>
       </c>
       <c r="G8">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H8" t="s">
         <v>78</v>
@@ -7567,7 +7570,7 @@
         <v>66</v>
       </c>
       <c r="G9">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H9" t="s">
         <v>78</v>
@@ -7629,7 +7632,7 @@
         <v>77</v>
       </c>
       <c r="G10">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H10" t="s">
         <v>78</v>
@@ -7691,7 +7694,7 @@
         <v>24</v>
       </c>
       <c r="G11">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H11" t="s">
         <v>78</v>
@@ -7753,7 +7756,7 @@
         <v>66</v>
       </c>
       <c r="G12">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H12" t="s">
         <v>78</v>
@@ -7815,7 +7818,7 @@
         <v>135</v>
       </c>
       <c r="G13">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H13" t="s">
         <v>25</v>
@@ -7871,7 +7874,7 @@
         <v>47</v>
       </c>
       <c r="G14">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H14" t="s">
         <v>25</v>
@@ -7927,7 +7930,7 @@
         <v>24</v>
       </c>
       <c r="G15">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H15" t="s">
         <v>25</v>
@@ -8039,7 +8042,7 @@
         <v>36</v>
       </c>
       <c r="G17">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H17" t="s">
         <v>25</v>
@@ -8095,7 +8098,7 @@
         <v>24</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H18" t="s">
         <v>25</v>
@@ -8151,7 +8154,7 @@
         <v>24</v>
       </c>
       <c r="G19">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H19" t="s">
         <v>25</v>
@@ -8207,7 +8210,7 @@
         <v>24</v>
       </c>
       <c r="G20">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H20" t="s">
         <v>25</v>
@@ -8263,7 +8266,7 @@
         <v>135</v>
       </c>
       <c r="G21">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H21" t="s">
         <v>25</v>
@@ -8319,7 +8322,7 @@
         <v>77</v>
       </c>
       <c r="G22">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H22" t="s">
         <v>25</v>
@@ -8375,7 +8378,7 @@
         <v>66</v>
       </c>
       <c r="G23">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H23" t="s">
         <v>25</v>
@@ -8431,7 +8434,7 @@
         <v>77</v>
       </c>
       <c r="G24">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H24" t="s">
         <v>78</v>
@@ -8493,7 +8496,7 @@
         <v>24</v>
       </c>
       <c r="G25">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H25" t="s">
         <v>78</v>
@@ -8555,7 +8558,7 @@
         <v>36</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H26" t="s">
         <v>78</v>
@@ -8617,7 +8620,7 @@
         <v>24</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H27" t="s">
         <v>78</v>
@@ -8679,7 +8682,7 @@
         <v>24</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H28" t="s">
         <v>78</v>
@@ -8691,7 +8694,7 @@
         <v>229</v>
       </c>
       <c r="K28">
-        <v>16</v>
+        <v>2022</v>
       </c>
       <c r="L28" t="s">
         <v>244</v>
@@ -8741,7 +8744,7 @@
         <v>24</v>
       </c>
       <c r="G29">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H29" t="s">
         <v>78</v>
@@ -8803,7 +8806,7 @@
         <v>36</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H30" t="s">
         <v>78</v>
@@ -8814,8 +8817,8 @@
       <c r="J30" t="s">
         <v>80</v>
       </c>
-      <c r="K30" t="s">
-        <v>26</v>
+      <c r="K30">
+        <v>2023</v>
       </c>
       <c r="L30" t="s">
         <v>256</v>
@@ -8865,7 +8868,7 @@
         <v>135</v>
       </c>
       <c r="G31">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H31" t="s">
         <v>78</v>
@@ -8927,7 +8930,7 @@
         <v>135</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H32" t="s">
         <v>78</v>
@@ -8989,7 +8992,7 @@
         <v>24</v>
       </c>
       <c r="G33">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H33" t="s">
         <v>78</v>
@@ -9051,7 +9054,7 @@
         <v>24</v>
       </c>
       <c r="G34">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H34" t="s">
         <v>78</v>
@@ -9113,7 +9116,7 @@
         <v>77</v>
       </c>
       <c r="G35">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H35" t="s">
         <v>78</v>
@@ -9175,7 +9178,7 @@
         <v>66</v>
       </c>
       <c r="G36">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H36" t="s">
         <v>78</v>
@@ -9237,7 +9240,7 @@
         <v>77</v>
       </c>
       <c r="G37">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H37" t="s">
         <v>78</v>
@@ -9248,8 +9251,8 @@
       <c r="J37" t="s">
         <v>80</v>
       </c>
-      <c r="K37" t="s">
-        <v>26</v>
+      <c r="K37">
+        <v>2023</v>
       </c>
       <c r="L37" t="s">
         <v>305</v>
@@ -9299,7 +9302,7 @@
         <v>47</v>
       </c>
       <c r="G38">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H38" t="s">
         <v>25</v>
@@ -9355,7 +9358,7 @@
         <v>77</v>
       </c>
       <c r="G39">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H39" t="s">
         <v>78</v>
@@ -9417,7 +9420,7 @@
         <v>66</v>
       </c>
       <c r="G40">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H40" t="s">
         <v>78</v>
@@ -9479,7 +9482,7 @@
         <v>36</v>
       </c>
       <c r="G41">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H41" t="s">
         <v>78</v>
@@ -9541,7 +9544,7 @@
         <v>24</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H42" t="s">
         <v>78</v>
@@ -9603,7 +9606,7 @@
         <v>77</v>
       </c>
       <c r="G43">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H43" t="s">
         <v>78</v>
@@ -9665,7 +9668,7 @@
         <v>47</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H44" t="s">
         <v>78</v>
@@ -9677,7 +9680,7 @@
         <v>80</v>
       </c>
       <c r="K44">
-        <v>19</v>
+        <v>2022</v>
       </c>
       <c r="L44" t="s">
         <v>353</v>
@@ -9727,7 +9730,7 @@
         <v>36</v>
       </c>
       <c r="G45">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H45" t="s">
         <v>78</v>
@@ -9789,7 +9792,7 @@
         <v>36</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H46" t="s">
         <v>78</v>
@@ -9851,7 +9854,7 @@
         <v>135</v>
       </c>
       <c r="G47">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H47" t="s">
         <v>78</v>
@@ -9913,7 +9916,7 @@
         <v>77</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H48" t="s">
         <v>78</v>
@@ -9975,7 +9978,7 @@
         <v>66</v>
       </c>
       <c r="G49">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H49" t="s">
         <v>78</v>
@@ -10037,7 +10040,7 @@
         <v>57</v>
       </c>
       <c r="G50">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H50" t="s">
         <v>78</v>
@@ -10099,7 +10102,7 @@
         <v>77</v>
       </c>
       <c r="G51">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H51" t="s">
         <v>78</v>
@@ -10161,7 +10164,7 @@
         <v>36</v>
       </c>
       <c r="G52">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H52" t="s">
         <v>78</v>
@@ -10223,7 +10226,7 @@
         <v>135</v>
       </c>
       <c r="G53">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H53" t="s">
         <v>78</v>
@@ -10285,7 +10288,7 @@
         <v>47</v>
       </c>
       <c r="G54">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H54" t="s">
         <v>78</v>
@@ -10347,7 +10350,7 @@
         <v>47</v>
       </c>
       <c r="G55">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H55" t="s">
         <v>78</v>
@@ -10409,7 +10412,7 @@
         <v>24</v>
       </c>
       <c r="G56">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H56" t="s">
         <v>78</v>
@@ -10471,7 +10474,7 @@
         <v>77</v>
       </c>
       <c r="G57">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H57" t="s">
         <v>78</v>
@@ -10533,7 +10536,7 @@
         <v>57</v>
       </c>
       <c r="G58">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H58" t="s">
         <v>25</v>
@@ -10589,7 +10592,7 @@
         <v>36</v>
       </c>
       <c r="G59">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H59" t="s">
         <v>78</v>
@@ -10651,7 +10654,7 @@
         <v>47</v>
       </c>
       <c r="G60">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H60" t="s">
         <v>78</v>
@@ -10662,8 +10665,8 @@
       <c r="J60" t="s">
         <v>80</v>
       </c>
-      <c r="K60" t="s">
-        <v>26</v>
+      <c r="K60">
+        <v>2023</v>
       </c>
       <c r="L60" t="s">
         <v>454</v>
@@ -10713,7 +10716,7 @@
         <v>47</v>
       </c>
       <c r="G61">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H61" t="s">
         <v>25</v>
@@ -10769,7 +10772,7 @@
         <v>77</v>
       </c>
       <c r="G62">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H62" t="s">
         <v>78</v>
@@ -10831,7 +10834,7 @@
         <v>135</v>
       </c>
       <c r="G63">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H63" t="s">
         <v>78</v>
@@ -10893,7 +10896,7 @@
         <v>24</v>
       </c>
       <c r="G64">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H64" t="s">
         <v>78</v>
@@ -10955,7 +10958,7 @@
         <v>36</v>
       </c>
       <c r="G65">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H65" t="s">
         <v>78</v>
@@ -11017,7 +11020,7 @@
         <v>77</v>
       </c>
       <c r="G66">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H66" t="s">
         <v>78</v>
@@ -11079,7 +11082,7 @@
         <v>66</v>
       </c>
       <c r="G67">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H67" t="s">
         <v>78</v>
@@ -11141,7 +11144,7 @@
         <v>77</v>
       </c>
       <c r="G68">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H68" t="s">
         <v>78</v>
@@ -11203,7 +11206,7 @@
         <v>66</v>
       </c>
       <c r="G69">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H69" t="s">
         <v>78</v>
@@ -11265,7 +11268,7 @@
         <v>24</v>
       </c>
       <c r="G70">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H70" t="s">
         <v>78</v>
@@ -11327,7 +11330,7 @@
         <v>77</v>
       </c>
       <c r="G71">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H71" t="s">
         <v>78</v>
@@ -11389,7 +11392,7 @@
         <v>135</v>
       </c>
       <c r="G72">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H72" t="s">
         <v>78</v>
@@ -11451,7 +11454,7 @@
         <v>36</v>
       </c>
       <c r="G73">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H73" t="s">
         <v>78</v>
@@ -11463,7 +11466,7 @@
         <v>229</v>
       </c>
       <c r="K73">
-        <v>22</v>
+        <v>2022</v>
       </c>
       <c r="L73" t="s">
         <v>528</v>
@@ -11513,7 +11516,7 @@
         <v>77</v>
       </c>
       <c r="G74">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H74" t="s">
         <v>78</v>
@@ -11575,7 +11578,7 @@
         <v>66</v>
       </c>
       <c r="G75">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H75" t="s">
         <v>78</v>
@@ -11637,7 +11640,7 @@
         <v>66</v>
       </c>
       <c r="G76">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H76" t="s">
         <v>78</v>
@@ -11699,7 +11702,7 @@
         <v>135</v>
       </c>
       <c r="G77">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H77" t="s">
         <v>78</v>
@@ -11761,7 +11764,7 @@
         <v>47</v>
       </c>
       <c r="G78">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H78" t="s">
         <v>78</v>
@@ -11823,7 +11826,7 @@
         <v>66</v>
       </c>
       <c r="G79">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H79" t="s">
         <v>78</v>
@@ -11885,7 +11888,7 @@
         <v>135</v>
       </c>
       <c r="G80">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H80" t="s">
         <v>78</v>
@@ -11947,7 +11950,7 @@
         <v>135</v>
       </c>
       <c r="G81">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H81" t="s">
         <v>78</v>
@@ -11958,8 +11961,8 @@
       <c r="J81" t="s">
         <v>229</v>
       </c>
-      <c r="K81" t="s">
-        <v>26</v>
+      <c r="K81">
+        <v>2023</v>
       </c>
       <c r="L81" t="s">
         <v>569</v>
@@ -12009,7 +12012,7 @@
         <v>47</v>
       </c>
       <c r="G82">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H82" t="s">
         <v>78</v>
@@ -12071,7 +12074,7 @@
         <v>77</v>
       </c>
       <c r="G83">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H83" t="s">
         <v>78</v>
@@ -12133,7 +12136,7 @@
         <v>66</v>
       </c>
       <c r="G84">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H84" t="s">
         <v>25</v>
@@ -12189,7 +12192,7 @@
         <v>36</v>
       </c>
       <c r="G85">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H85" t="s">
         <v>78</v>
@@ -12200,8 +12203,8 @@
       <c r="J85" t="s">
         <v>229</v>
       </c>
-      <c r="K85" t="s">
-        <v>26</v>
+      <c r="K85">
+        <v>2023</v>
       </c>
       <c r="L85" t="s">
         <v>594</v>
@@ -12251,7 +12254,7 @@
         <v>66</v>
       </c>
       <c r="G86">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H86" t="s">
         <v>25</v>
@@ -12307,7 +12310,7 @@
         <v>24</v>
       </c>
       <c r="G87">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H87" t="s">
         <v>78</v>
@@ -12369,7 +12372,7 @@
         <v>135</v>
       </c>
       <c r="G88">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H88" t="s">
         <v>78</v>
@@ -12431,7 +12434,7 @@
         <v>24</v>
       </c>
       <c r="G89">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H89" t="s">
         <v>78</v>
@@ -12443,7 +12446,7 @@
         <v>80</v>
       </c>
       <c r="K89">
-        <v>8</v>
+        <v>2022</v>
       </c>
       <c r="L89" t="s">
         <v>620</v>
@@ -12493,7 +12496,7 @@
         <v>135</v>
       </c>
       <c r="G90">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H90" t="s">
         <v>78</v>
@@ -12555,7 +12558,7 @@
         <v>24</v>
       </c>
       <c r="G91">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H91" t="s">
         <v>78</v>
@@ -12617,7 +12620,7 @@
         <v>66</v>
       </c>
       <c r="G92">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H92" t="s">
         <v>78</v>
@@ -12679,7 +12682,7 @@
         <v>36</v>
       </c>
       <c r="G93">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H93" t="s">
         <v>78</v>
@@ -12741,7 +12744,7 @@
         <v>77</v>
       </c>
       <c r="G94">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H94" t="s">
         <v>78</v>
@@ -12803,7 +12806,7 @@
         <v>36</v>
       </c>
       <c r="G95">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H95" t="s">
         <v>78</v>
@@ -12865,7 +12868,7 @@
         <v>36</v>
       </c>
       <c r="G96">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H96" t="s">
         <v>78</v>
@@ -12927,7 +12930,7 @@
         <v>66</v>
       </c>
       <c r="G97">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H97" t="s">
         <v>78</v>
@@ -12989,7 +12992,7 @@
         <v>24</v>
       </c>
       <c r="G98">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H98" t="s">
         <v>78</v>
@@ -13051,7 +13054,7 @@
         <v>24</v>
       </c>
       <c r="G99">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H99" t="s">
         <v>78</v>
@@ -13113,7 +13116,7 @@
         <v>77</v>
       </c>
       <c r="G100">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H100" t="s">
         <v>78</v>
@@ -13175,7 +13178,7 @@
         <v>77</v>
       </c>
       <c r="G101">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H101" t="s">
         <v>25</v>
@@ -13231,7 +13234,7 @@
         <v>66</v>
       </c>
       <c r="G102">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H102" t="s">
         <v>25</v>
@@ -13287,7 +13290,7 @@
         <v>36</v>
       </c>
       <c r="G103">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H103" t="s">
         <v>25</v>
@@ -13343,7 +13346,7 @@
         <v>24</v>
       </c>
       <c r="G104">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H104" t="s">
         <v>25</v>
@@ -13399,7 +13402,7 @@
         <v>36</v>
       </c>
       <c r="G105">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H105" t="s">
         <v>25</v>
@@ -13455,7 +13458,7 @@
         <v>135</v>
       </c>
       <c r="G106">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H106" t="s">
         <v>25</v>
@@ -13511,7 +13514,7 @@
         <v>36</v>
       </c>
       <c r="G107">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H107" t="s">
         <v>25</v>
@@ -13567,7 +13570,7 @@
         <v>66</v>
       </c>
       <c r="G108">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H108" t="s">
         <v>25</v>
@@ -13623,7 +13626,7 @@
         <v>36</v>
       </c>
       <c r="G109">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H109" t="s">
         <v>78</v>
@@ -13685,7 +13688,7 @@
         <v>77</v>
       </c>
       <c r="G110">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H110" t="s">
         <v>78</v>
@@ -13747,7 +13750,7 @@
         <v>36</v>
       </c>
       <c r="G111">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H111" t="s">
         <v>78</v>
@@ -13809,7 +13812,7 @@
         <v>77</v>
       </c>
       <c r="G112">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H112" t="s">
         <v>78</v>
@@ -13871,7 +13874,7 @@
         <v>36</v>
       </c>
       <c r="G113">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H113" t="s">
         <v>78</v>
@@ -13933,7 +13936,7 @@
         <v>135</v>
       </c>
       <c r="G114">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H114" t="s">
         <v>78</v>
@@ -13995,7 +13998,7 @@
         <v>57</v>
       </c>
       <c r="G115">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H115" t="s">
         <v>25</v>
@@ -14051,7 +14054,7 @@
         <v>36</v>
       </c>
       <c r="G116">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H116" t="s">
         <v>25</v>
@@ -14107,7 +14110,7 @@
         <v>135</v>
       </c>
       <c r="G117">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H117" t="s">
         <v>78</v>
@@ -14119,7 +14122,7 @@
         <v>229</v>
       </c>
       <c r="K117">
-        <v>12</v>
+        <v>2022</v>
       </c>
       <c r="L117" t="s">
         <v>778</v>
@@ -14169,7 +14172,7 @@
         <v>77</v>
       </c>
       <c r="G118">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H118" t="s">
         <v>78</v>
@@ -14231,7 +14234,7 @@
         <v>66</v>
       </c>
       <c r="G119">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H119" t="s">
         <v>78</v>
@@ -14293,7 +14296,7 @@
         <v>135</v>
       </c>
       <c r="G120">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H120" t="s">
         <v>78</v>
@@ -14304,8 +14307,8 @@
       <c r="J120" t="s">
         <v>229</v>
       </c>
-      <c r="K120" t="s">
-        <v>26</v>
+      <c r="K120">
+        <v>2022</v>
       </c>
       <c r="L120" t="s">
         <v>796</v>
@@ -14355,7 +14358,7 @@
         <v>57</v>
       </c>
       <c r="G121">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H121" t="s">
         <v>78</v>
@@ -14417,7 +14420,7 @@
         <v>77</v>
       </c>
       <c r="G122">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H122" t="s">
         <v>78</v>
@@ -14479,7 +14482,7 @@
         <v>36</v>
       </c>
       <c r="G123">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H123" t="s">
         <v>78</v>
@@ -14541,7 +14544,7 @@
         <v>77</v>
       </c>
       <c r="G124">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H124" t="s">
         <v>78</v>
@@ -14603,7 +14606,7 @@
         <v>36</v>
       </c>
       <c r="G125">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H125" t="s">
         <v>78</v>
@@ -14665,7 +14668,7 @@
         <v>36</v>
       </c>
       <c r="G126">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H126" t="s">
         <v>78</v>
@@ -14727,7 +14730,7 @@
         <v>77</v>
       </c>
       <c r="G127">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H127" t="s">
         <v>78</v>
@@ -14789,7 +14792,7 @@
         <v>36</v>
       </c>
       <c r="G128">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H128" t="s">
         <v>78</v>
@@ -14851,7 +14854,7 @@
         <v>66</v>
       </c>
       <c r="G129">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H129" t="s">
         <v>78</v>
@@ -14913,7 +14916,7 @@
         <v>36</v>
       </c>
       <c r="G130">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H130" t="s">
         <v>78</v>
@@ -14975,7 +14978,7 @@
         <v>24</v>
       </c>
       <c r="G131">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H131" t="s">
         <v>25</v>
@@ -15031,7 +15034,7 @@
         <v>135</v>
       </c>
       <c r="G132">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H132" t="s">
         <v>78</v>
@@ -15093,7 +15096,7 @@
         <v>47</v>
       </c>
       <c r="G133">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H133" t="s">
         <v>78</v>
@@ -15155,7 +15158,7 @@
         <v>135</v>
       </c>
       <c r="G134">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H134" t="s">
         <v>78</v>
@@ -15217,7 +15220,7 @@
         <v>36</v>
       </c>
       <c r="G135">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H135" t="s">
         <v>78</v>
@@ -15279,7 +15282,7 @@
         <v>36</v>
       </c>
       <c r="G136">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H136" t="s">
         <v>78</v>
@@ -15320,7 +15323,7 @@
         <v>24</v>
       </c>
       <c r="G137">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H137" t="s">
         <v>78</v>
@@ -15382,7 +15385,7 @@
         <v>36</v>
       </c>
       <c r="G138">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H138" t="s">
         <v>78</v>
@@ -15444,7 +15447,7 @@
         <v>77</v>
       </c>
       <c r="G139">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H139" t="s">
         <v>78</v>
@@ -15456,7 +15459,7 @@
         <v>80</v>
       </c>
       <c r="K139">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="L139" t="s">
         <v>903</v>
@@ -15506,7 +15509,7 @@
         <v>36</v>
       </c>
       <c r="G140">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H140" t="s">
         <v>78</v>
@@ -15568,7 +15571,7 @@
         <v>135</v>
       </c>
       <c r="G141">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H141" t="s">
         <v>78</v>
@@ -15630,7 +15633,7 @@
         <v>24</v>
       </c>
       <c r="G142">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H142" t="s">
         <v>78</v>
@@ -15692,7 +15695,7 @@
         <v>77</v>
       </c>
       <c r="G143">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H143" t="s">
         <v>78</v>
@@ -15754,7 +15757,7 @@
         <v>24</v>
       </c>
       <c r="G144">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H144" t="s">
         <v>78</v>
@@ -15816,7 +15819,7 @@
         <v>77</v>
       </c>
       <c r="G145">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H145" t="s">
         <v>78</v>
@@ -15878,7 +15881,7 @@
         <v>77</v>
       </c>
       <c r="G146">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H146" t="s">
         <v>78</v>
@@ -15940,7 +15943,7 @@
         <v>24</v>
       </c>
       <c r="G147">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H147" t="s">
         <v>78</v>
@@ -16002,7 +16005,7 @@
         <v>24</v>
       </c>
       <c r="G148">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H148" t="s">
         <v>78</v>
@@ -16013,8 +16016,8 @@
       <c r="J148" t="s">
         <v>229</v>
       </c>
-      <c r="K148" t="s">
-        <v>26</v>
+      <c r="K148">
+        <v>2023</v>
       </c>
       <c r="L148" t="s">
         <v>959</v>
@@ -16064,7 +16067,7 @@
         <v>47</v>
       </c>
       <c r="G149">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H149" t="s">
         <v>78</v>
@@ -16075,8 +16078,8 @@
       <c r="J149" t="s">
         <v>229</v>
       </c>
-      <c r="K149" t="s">
-        <v>26</v>
+      <c r="K149">
+        <v>2023</v>
       </c>
       <c r="L149" t="s">
         <v>965</v>
@@ -16126,7 +16129,7 @@
         <v>135</v>
       </c>
       <c r="G150">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H150" t="s">
         <v>78</v>
@@ -16188,7 +16191,7 @@
         <v>66</v>
       </c>
       <c r="G151">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H151" t="s">
         <v>78</v>
@@ -16199,8 +16202,8 @@
       <c r="J151" t="s">
         <v>229</v>
       </c>
-      <c r="K151" t="s">
-        <v>26</v>
+      <c r="K151">
+        <v>2023</v>
       </c>
       <c r="L151" t="s">
         <v>974</v>
@@ -16250,7 +16253,7 @@
         <v>24</v>
       </c>
       <c r="G152">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H152" t="s">
         <v>25</v>
@@ -16306,7 +16309,7 @@
         <v>66</v>
       </c>
       <c r="G153">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H153" t="s">
         <v>25</v>
@@ -16362,7 +16365,7 @@
         <v>135</v>
       </c>
       <c r="G154">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H154" t="s">
         <v>78</v>
@@ -16424,7 +16427,7 @@
         <v>77</v>
       </c>
       <c r="G155">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H155" t="s">
         <v>78</v>
@@ -16486,7 +16489,7 @@
         <v>24</v>
       </c>
       <c r="G156">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H156" t="s">
         <v>78</v>
@@ -16548,7 +16551,7 @@
         <v>24</v>
       </c>
       <c r="G157">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H157" t="s">
         <v>78</v>
@@ -16610,7 +16613,7 @@
         <v>135</v>
       </c>
       <c r="G158">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H158" t="s">
         <v>78</v>
@@ -16672,7 +16675,7 @@
         <v>36</v>
       </c>
       <c r="G159">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H159" t="s">
         <v>78</v>
@@ -16734,7 +16737,7 @@
         <v>24</v>
       </c>
       <c r="G160">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H160" t="s">
         <v>78</v>
@@ -16796,7 +16799,7 @@
         <v>36</v>
       </c>
       <c r="G161">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H161" t="s">
         <v>78</v>
@@ -16858,7 +16861,7 @@
         <v>57</v>
       </c>
       <c r="G162">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H162" t="s">
         <v>78</v>
@@ -16920,7 +16923,7 @@
         <v>57</v>
       </c>
       <c r="G163">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H163" t="s">
         <v>25</v>
@@ -16976,7 +16979,7 @@
         <v>36</v>
       </c>
       <c r="G164">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H164" t="s">
         <v>78</v>
@@ -17038,7 +17041,7 @@
         <v>24</v>
       </c>
       <c r="G165">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H165" t="s">
         <v>78</v>
@@ -17100,7 +17103,7 @@
         <v>66</v>
       </c>
       <c r="G166">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H166" t="s">
         <v>78</v>
@@ -17162,7 +17165,7 @@
         <v>66</v>
       </c>
       <c r="G167">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H167" t="s">
         <v>78</v>
@@ -17224,7 +17227,7 @@
         <v>77</v>
       </c>
       <c r="G168">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H168" t="s">
         <v>25</v>
@@ -17280,13 +17283,13 @@
         <v>47</v>
       </c>
       <c r="G169">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H169" t="s">
         <v>25</v>
       </c>
-      <c r="K169" t="s">
-        <v>26</v>
+      <c r="K169">
+        <v>2023</v>
       </c>
       <c r="L169" t="s">
         <v>1070</v>
@@ -17336,7 +17339,7 @@
         <v>24</v>
       </c>
       <c r="G170">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H170" t="s">
         <v>78</v>
@@ -17398,7 +17401,7 @@
         <v>24</v>
       </c>
       <c r="G171">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H171" t="s">
         <v>78</v>
@@ -17460,7 +17463,7 @@
         <v>77</v>
       </c>
       <c r="G172">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H172" t="s">
         <v>78</v>
@@ -17522,7 +17525,7 @@
         <v>57</v>
       </c>
       <c r="G173">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H173" t="s">
         <v>78</v>
@@ -17584,7 +17587,7 @@
         <v>36</v>
       </c>
       <c r="G174">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H174" t="s">
         <v>78</v>
@@ -17595,8 +17598,8 @@
       <c r="J174" t="s">
         <v>229</v>
       </c>
-      <c r="K174" t="s">
-        <v>26</v>
+      <c r="K174">
+        <v>2023</v>
       </c>
       <c r="L174" t="s">
         <v>1093</v>
@@ -17646,7 +17649,7 @@
         <v>24</v>
       </c>
       <c r="G175">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H175" t="s">
         <v>78</v>
@@ -17708,7 +17711,7 @@
         <v>47</v>
       </c>
       <c r="G176">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H176" t="s">
         <v>25</v>
@@ -17764,7 +17767,7 @@
         <v>135</v>
       </c>
       <c r="G177">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H177" t="s">
         <v>78</v>
@@ -17826,7 +17829,7 @@
         <v>135</v>
       </c>
       <c r="G178">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H178" t="s">
         <v>25</v>
@@ -17882,7 +17885,7 @@
         <v>24</v>
       </c>
       <c r="G179">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H179" t="s">
         <v>25</v>
@@ -17938,7 +17941,7 @@
         <v>47</v>
       </c>
       <c r="G180">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H180" t="s">
         <v>25</v>
@@ -17994,7 +17997,7 @@
         <v>135</v>
       </c>
       <c r="G181">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H181" t="s">
         <v>78</v>
@@ -18056,7 +18059,7 @@
         <v>66</v>
       </c>
       <c r="G182">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H182" t="s">
         <v>78</v>
@@ -18118,7 +18121,7 @@
         <v>66</v>
       </c>
       <c r="G183">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H183" t="s">
         <v>78</v>
@@ -18180,7 +18183,7 @@
         <v>77</v>
       </c>
       <c r="G184">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H184" t="s">
         <v>78</v>
@@ -18191,8 +18194,8 @@
       <c r="J184" t="s">
         <v>229</v>
       </c>
-      <c r="K184" t="s">
-        <v>26</v>
+      <c r="K184">
+        <v>2023</v>
       </c>
       <c r="L184" t="s">
         <v>1137</v>
@@ -18242,7 +18245,7 @@
         <v>66</v>
       </c>
       <c r="G185">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H185" t="s">
         <v>78</v>
@@ -18304,7 +18307,7 @@
         <v>77</v>
       </c>
       <c r="G186">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H186" t="s">
         <v>78</v>
@@ -18316,7 +18319,7 @@
         <v>80</v>
       </c>
       <c r="K186">
-        <v>14</v>
+        <v>2022</v>
       </c>
       <c r="L186" t="s">
         <v>1148</v>
@@ -18366,7 +18369,7 @@
         <v>36</v>
       </c>
       <c r="G187">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H187" t="s">
         <v>78</v>
@@ -18428,7 +18431,7 @@
         <v>36</v>
       </c>
       <c r="G188">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H188" t="s">
         <v>78</v>
@@ -18439,8 +18442,8 @@
       <c r="J188" t="s">
         <v>80</v>
       </c>
-      <c r="K188" t="s">
-        <v>26</v>
+      <c r="K188">
+        <v>2023</v>
       </c>
       <c r="L188" t="s">
         <v>1160</v>
@@ -18490,7 +18493,7 @@
         <v>24</v>
       </c>
       <c r="G189">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H189" t="s">
         <v>78</v>
@@ -18552,7 +18555,7 @@
         <v>47</v>
       </c>
       <c r="G190">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H190" t="s">
         <v>78</v>
@@ -18614,7 +18617,7 @@
         <v>135</v>
       </c>
       <c r="G191">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H191" t="s">
         <v>78</v>
@@ -18676,7 +18679,7 @@
         <v>24</v>
       </c>
       <c r="G192">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H192" t="s">
         <v>78</v>
@@ -18738,7 +18741,7 @@
         <v>66</v>
       </c>
       <c r="G193">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H193" t="s">
         <v>78</v>
@@ -18800,7 +18803,7 @@
         <v>36</v>
       </c>
       <c r="G194">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H194" t="s">
         <v>78</v>
@@ -18811,8 +18814,8 @@
       <c r="J194" t="s">
         <v>229</v>
       </c>
-      <c r="K194" t="s">
-        <v>26</v>
+      <c r="K194">
+        <v>2023</v>
       </c>
       <c r="L194" t="s">
         <v>1187</v>
@@ -18862,7 +18865,7 @@
         <v>77</v>
       </c>
       <c r="G195">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H195" t="s">
         <v>78</v>
@@ -18924,7 +18927,7 @@
         <v>66</v>
       </c>
       <c r="G196">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H196" t="s">
         <v>78</v>
@@ -18986,7 +18989,7 @@
         <v>36</v>
       </c>
       <c r="G197">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H197" t="s">
         <v>78</v>
@@ -19048,7 +19051,7 @@
         <v>24</v>
       </c>
       <c r="G198">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H198" t="s">
         <v>78</v>
@@ -19110,7 +19113,7 @@
         <v>66</v>
       </c>
       <c r="G199">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H199" t="s">
         <v>78</v>
@@ -19172,7 +19175,7 @@
         <v>77</v>
       </c>
       <c r="G200">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H200" t="s">
         <v>78</v>
@@ -19234,7 +19237,7 @@
         <v>77</v>
       </c>
       <c r="G201">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H201" t="s">
         <v>78</v>
@@ -19296,7 +19299,7 @@
         <v>135</v>
       </c>
       <c r="G202">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H202" t="s">
         <v>78</v>
@@ -19358,7 +19361,7 @@
         <v>135</v>
       </c>
       <c r="G203">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H203" t="s">
         <v>78</v>
@@ -19420,7 +19423,7 @@
         <v>77</v>
       </c>
       <c r="G204">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H204" t="s">
         <v>78</v>
@@ -19482,7 +19485,7 @@
         <v>135</v>
       </c>
       <c r="G205">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H205" t="s">
         <v>78</v>
@@ -19544,7 +19547,7 @@
         <v>24</v>
       </c>
       <c r="G206">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H206" t="s">
         <v>78</v>
@@ -19606,7 +19609,7 @@
         <v>135</v>
       </c>
       <c r="G207">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H207" t="s">
         <v>78</v>
@@ -19668,7 +19671,7 @@
         <v>77</v>
       </c>
       <c r="G208">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H208" t="s">
         <v>78</v>
@@ -19730,7 +19733,7 @@
         <v>77</v>
       </c>
       <c r="G209">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H209" t="s">
         <v>78</v>
@@ -19792,7 +19795,7 @@
         <v>57</v>
       </c>
       <c r="G210">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H210" t="s">
         <v>78</v>
@@ -19854,7 +19857,7 @@
         <v>135</v>
       </c>
       <c r="G211">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H211" t="s">
         <v>78</v>
@@ -19916,7 +19919,7 @@
         <v>77</v>
       </c>
       <c r="G212">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H212" t="s">
         <v>78</v>
@@ -19978,7 +19981,7 @@
         <v>66</v>
       </c>
       <c r="G213">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H213" t="s">
         <v>78</v>
@@ -20040,7 +20043,7 @@
         <v>135</v>
       </c>
       <c r="G214">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H214" t="s">
         <v>78</v>
@@ -20102,7 +20105,7 @@
         <v>36</v>
       </c>
       <c r="G215">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H215" t="s">
         <v>78</v>
@@ -20114,7 +20117,7 @@
         <v>229</v>
       </c>
       <c r="K215">
-        <v>18</v>
+        <v>2022</v>
       </c>
       <c r="L215" t="s">
         <v>1304</v>
@@ -20164,7 +20167,7 @@
         <v>66</v>
       </c>
       <c r="G216">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H216" t="s">
         <v>78</v>
@@ -20226,7 +20229,7 @@
         <v>77</v>
       </c>
       <c r="G217">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H217" t="s">
         <v>78</v>
@@ -20238,7 +20241,7 @@
         <v>229</v>
       </c>
       <c r="K217">
-        <v>6</v>
+        <v>2022</v>
       </c>
       <c r="L217" t="s">
         <v>1265</v>
@@ -20288,7 +20291,7 @@
         <v>24</v>
       </c>
       <c r="G218">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H218" t="s">
         <v>78</v>
@@ -20350,7 +20353,7 @@
         <v>66</v>
       </c>
       <c r="G219">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H219" t="s">
         <v>78</v>
@@ -20412,7 +20415,7 @@
         <v>77</v>
       </c>
       <c r="G220">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H220" t="s">
         <v>78</v>
@@ -20474,7 +20477,7 @@
         <v>24</v>
       </c>
       <c r="G221">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H221" t="s">
         <v>78</v>
@@ -20536,7 +20539,7 @@
         <v>66</v>
       </c>
       <c r="G222">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H222" t="s">
         <v>78</v>
@@ -20598,7 +20601,7 @@
         <v>77</v>
       </c>
       <c r="G223">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H223" t="s">
         <v>78</v>
@@ -20660,7 +20663,7 @@
         <v>66</v>
       </c>
       <c r="G224">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H224" t="s">
         <v>78</v>
@@ -20722,7 +20725,7 @@
         <v>57</v>
       </c>
       <c r="G225">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H225" t="s">
         <v>78</v>
@@ -20784,7 +20787,7 @@
         <v>24</v>
       </c>
       <c r="G226">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H226" t="s">
         <v>78</v>
@@ -20846,7 +20849,7 @@
         <v>36</v>
       </c>
       <c r="G227">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H227" t="s">
         <v>78</v>
@@ -20908,7 +20911,7 @@
         <v>77</v>
       </c>
       <c r="G228">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H228" t="s">
         <v>78</v>
@@ -20970,7 +20973,7 @@
         <v>66</v>
       </c>
       <c r="G229">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H229" t="s">
         <v>78</v>
@@ -20982,7 +20985,7 @@
         <v>80</v>
       </c>
       <c r="K229">
-        <v>3</v>
+        <v>2022</v>
       </c>
       <c r="L229" t="s">
         <v>1376</v>
@@ -21032,7 +21035,7 @@
         <v>77</v>
       </c>
       <c r="G230">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H230" t="s">
         <v>78</v>
@@ -21094,7 +21097,7 @@
         <v>66</v>
       </c>
       <c r="G231">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H231" t="s">
         <v>78</v>
@@ -21135,7 +21138,7 @@
         <v>77</v>
       </c>
       <c r="G232">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H232" t="s">
         <v>78</v>
@@ -21197,7 +21200,7 @@
         <v>66</v>
       </c>
       <c r="G233">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H233" t="s">
         <v>78</v>
@@ -21259,7 +21262,7 @@
         <v>57</v>
       </c>
       <c r="G234">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H234" t="s">
         <v>78</v>
@@ -21270,8 +21273,8 @@
       <c r="J234" t="s">
         <v>229</v>
       </c>
-      <c r="K234" t="s">
-        <v>26</v>
+      <c r="K234">
+        <v>2023</v>
       </c>
       <c r="L234" t="s">
         <v>1402</v>
@@ -21321,7 +21324,7 @@
         <v>24</v>
       </c>
       <c r="G235">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H235" t="s">
         <v>78</v>
@@ -21333,7 +21336,7 @@
         <v>80</v>
       </c>
       <c r="K235">
-        <v>7</v>
+        <v>2022</v>
       </c>
       <c r="L235" t="s">
         <v>1407</v>
@@ -21383,7 +21386,7 @@
         <v>135</v>
       </c>
       <c r="G236">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H236" t="s">
         <v>78</v>
@@ -21445,7 +21448,7 @@
         <v>24</v>
       </c>
       <c r="G237">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H237" t="s">
         <v>78</v>
@@ -21507,7 +21510,7 @@
         <v>77</v>
       </c>
       <c r="G238">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H238" t="s">
         <v>25</v>
@@ -21563,7 +21566,7 @@
         <v>57</v>
       </c>
       <c r="G239">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H239" t="s">
         <v>78</v>
@@ -21625,7 +21628,7 @@
         <v>66</v>
       </c>
       <c r="G240">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H240" t="s">
         <v>78</v>
@@ -21687,7 +21690,7 @@
         <v>77</v>
       </c>
       <c r="G241">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H241" t="s">
         <v>78</v>
@@ -21749,7 +21752,7 @@
         <v>66</v>
       </c>
       <c r="G242">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H242" t="s">
         <v>78</v>
@@ -21811,7 +21814,7 @@
         <v>36</v>
       </c>
       <c r="G243">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H243" t="s">
         <v>78</v>
@@ -21873,7 +21876,7 @@
         <v>36</v>
       </c>
       <c r="G244">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H244" t="s">
         <v>78</v>
@@ -21914,7 +21917,7 @@
         <v>135</v>
       </c>
       <c r="G245">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H245" t="s">
         <v>78</v>
@@ -21926,7 +21929,7 @@
         <v>80</v>
       </c>
       <c r="K245">
-        <v>2</v>
+        <v>2022</v>
       </c>
       <c r="L245" t="s">
         <v>1453</v>
@@ -21976,7 +21979,7 @@
         <v>24</v>
       </c>
       <c r="G246">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H246" t="s">
         <v>78</v>
@@ -22038,7 +22041,7 @@
         <v>66</v>
       </c>
       <c r="G247">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H247" t="s">
         <v>78</v>
@@ -22100,7 +22103,7 @@
         <v>24</v>
       </c>
       <c r="G248">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H248" t="s">
         <v>78</v>
@@ -22162,7 +22165,7 @@
         <v>24</v>
       </c>
       <c r="G249">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H249" t="s">
         <v>78</v>
@@ -22224,7 +22227,7 @@
         <v>77</v>
       </c>
       <c r="G250">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H250" t="s">
         <v>78</v>
@@ -22286,7 +22289,7 @@
         <v>47</v>
       </c>
       <c r="G251">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H251" t="s">
         <v>78</v>
@@ -22297,8 +22300,8 @@
       <c r="J251" t="s">
         <v>80</v>
       </c>
-      <c r="K251" t="s">
-        <v>26</v>
+      <c r="K251">
+        <v>2023</v>
       </c>
       <c r="L251" t="s">
         <v>1478</v>
@@ -22348,7 +22351,7 @@
         <v>47</v>
       </c>
       <c r="G252">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H252" t="s">
         <v>78</v>
@@ -22410,7 +22413,7 @@
         <v>77</v>
       </c>
       <c r="G253">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H253" t="s">
         <v>78</v>
@@ -22472,7 +22475,7 @@
         <v>24</v>
       </c>
       <c r="G254">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H254" t="s">
         <v>78</v>
@@ -22534,7 +22537,7 @@
         <v>57</v>
       </c>
       <c r="G255">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H255" t="s">
         <v>78</v>
@@ -22596,7 +22599,7 @@
         <v>47</v>
       </c>
       <c r="G256">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H256" t="s">
         <v>78</v>
@@ -22658,7 +22661,7 @@
         <v>66</v>
       </c>
       <c r="G257">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H257" t="s">
         <v>78</v>
@@ -22720,7 +22723,7 @@
         <v>24</v>
       </c>
       <c r="G258">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H258" t="s">
         <v>78</v>
@@ -22782,7 +22785,7 @@
         <v>24</v>
       </c>
       <c r="G259">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H259" t="s">
         <v>78</v>
@@ -22844,7 +22847,7 @@
         <v>36</v>
       </c>
       <c r="G260">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H260" t="s">
         <v>78</v>
@@ -22856,7 +22859,7 @@
         <v>229</v>
       </c>
       <c r="K260">
-        <v>24</v>
+        <v>2022</v>
       </c>
       <c r="L260" t="s">
         <v>1526</v>
@@ -22906,7 +22909,7 @@
         <v>77</v>
       </c>
       <c r="G261">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H261" t="s">
         <v>78</v>
@@ -22968,7 +22971,7 @@
         <v>135</v>
       </c>
       <c r="G262">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H262" t="s">
         <v>78</v>
@@ -23030,7 +23033,7 @@
         <v>66</v>
       </c>
       <c r="G263">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H263" t="s">
         <v>78</v>
@@ -23092,7 +23095,7 @@
         <v>77</v>
       </c>
       <c r="G264">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H264" t="s">
         <v>78</v>
@@ -23154,7 +23157,7 @@
         <v>77</v>
       </c>
       <c r="G265">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H265" t="s">
         <v>78</v>
@@ -23216,7 +23219,7 @@
         <v>24</v>
       </c>
       <c r="G266">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H266" t="s">
         <v>78</v>
@@ -23278,7 +23281,7 @@
         <v>77</v>
       </c>
       <c r="G267">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H267" t="s">
         <v>78</v>
@@ -23340,7 +23343,7 @@
         <v>24</v>
       </c>
       <c r="G268">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H268" t="s">
         <v>78</v>
@@ -23402,7 +23405,7 @@
         <v>24</v>
       </c>
       <c r="G269">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H269" t="s">
         <v>78</v>
@@ -23464,7 +23467,7 @@
         <v>66</v>
       </c>
       <c r="G270">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H270" t="s">
         <v>78</v>
@@ -23526,7 +23529,7 @@
         <v>36</v>
       </c>
       <c r="G271">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H271" t="s">
         <v>78</v>
@@ -23588,7 +23591,7 @@
         <v>47</v>
       </c>
       <c r="G272">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H272" t="s">
         <v>78</v>
@@ -23650,7 +23653,7 @@
         <v>77</v>
       </c>
       <c r="G273">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H273" t="s">
         <v>78</v>
@@ -23712,7 +23715,7 @@
         <v>135</v>
       </c>
       <c r="G274">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H274" t="s">
         <v>78</v>
@@ -23774,7 +23777,7 @@
         <v>77</v>
       </c>
       <c r="G275">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H275" t="s">
         <v>78</v>
@@ -23836,7 +23839,7 @@
         <v>24</v>
       </c>
       <c r="G276">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H276" t="s">
         <v>78</v>
@@ -23898,7 +23901,7 @@
         <v>77</v>
       </c>
       <c r="G277">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H277" t="s">
         <v>78</v>
@@ -23910,7 +23913,7 @@
         <v>80</v>
       </c>
       <c r="K277">
-        <v>15</v>
+        <v>2022</v>
       </c>
       <c r="L277" t="s">
         <v>1610</v>
@@ -23960,7 +23963,7 @@
         <v>24</v>
       </c>
       <c r="G278">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H278" t="s">
         <v>78</v>
@@ -24022,7 +24025,7 @@
         <v>57</v>
       </c>
       <c r="G279">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H279" t="s">
         <v>78</v>
@@ -24084,7 +24087,7 @@
         <v>66</v>
       </c>
       <c r="G280">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H280" t="s">
         <v>78</v>
@@ -24146,7 +24149,7 @@
         <v>135</v>
       </c>
       <c r="G281">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H281" t="s">
         <v>78</v>
@@ -24208,7 +24211,7 @@
         <v>77</v>
       </c>
       <c r="G282">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H282" t="s">
         <v>78</v>
@@ -24270,7 +24273,7 @@
         <v>66</v>
       </c>
       <c r="G283">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H283" t="s">
         <v>78</v>
@@ -24332,7 +24335,7 @@
         <v>36</v>
       </c>
       <c r="G284">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H284" t="s">
         <v>78</v>
@@ -24394,7 +24397,7 @@
         <v>77</v>
       </c>
       <c r="G285">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H285" t="s">
         <v>78</v>
@@ -24406,7 +24409,7 @@
         <v>229</v>
       </c>
       <c r="K285">
-        <v>4</v>
+        <v>2022</v>
       </c>
       <c r="L285" t="s">
         <v>1654</v>
@@ -24456,7 +24459,7 @@
         <v>47</v>
       </c>
       <c r="G286">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H286" t="s">
         <v>78</v>
@@ -24518,7 +24521,7 @@
         <v>24</v>
       </c>
       <c r="G287">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H287" t="s">
         <v>78</v>
@@ -24580,7 +24583,7 @@
         <v>77</v>
       </c>
       <c r="G288">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H288" t="s">
         <v>78</v>
@@ -24592,7 +24595,7 @@
         <v>229</v>
       </c>
       <c r="K288">
-        <v>5</v>
+        <v>2022</v>
       </c>
       <c r="L288" t="s">
         <v>1668</v>
@@ -24642,7 +24645,7 @@
         <v>36</v>
       </c>
       <c r="G289">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H289" t="s">
         <v>78</v>
@@ -24704,7 +24707,7 @@
         <v>24</v>
       </c>
       <c r="G290">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H290" t="s">
         <v>78</v>
@@ -24766,7 +24769,7 @@
         <v>24</v>
       </c>
       <c r="G291">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H291" t="s">
         <v>78</v>
@@ -24828,7 +24831,7 @@
         <v>47</v>
       </c>
       <c r="G292">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H292" t="s">
         <v>78</v>
@@ -24890,7 +24893,7 @@
         <v>66</v>
       </c>
       <c r="G293">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H293" t="s">
         <v>78</v>
@@ -24952,7 +24955,7 @@
         <v>24</v>
       </c>
       <c r="G294">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H294" t="s">
         <v>78</v>
@@ -25014,7 +25017,7 @@
         <v>66</v>
       </c>
       <c r="G295">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H295" t="s">
         <v>78</v>
@@ -25076,7 +25079,7 @@
         <v>77</v>
       </c>
       <c r="G296">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H296" t="s">
         <v>78</v>
@@ -25138,7 +25141,7 @@
         <v>47</v>
       </c>
       <c r="G297">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H297" t="s">
         <v>78</v>
@@ -25149,8 +25152,8 @@
       <c r="J297" t="s">
         <v>229</v>
       </c>
-      <c r="K297" t="s">
-        <v>26</v>
+      <c r="K297">
+        <v>2023</v>
       </c>
       <c r="L297" t="s">
         <v>460</v>
@@ -25200,7 +25203,7 @@
         <v>135</v>
       </c>
       <c r="G298">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H298" t="s">
         <v>78</v>
@@ -25262,7 +25265,7 @@
         <v>36</v>
       </c>
       <c r="G299">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H299" t="s">
         <v>78</v>
@@ -25324,7 +25327,7 @@
         <v>66</v>
       </c>
       <c r="G300">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H300" t="s">
         <v>78</v>
@@ -25386,7 +25389,7 @@
         <v>36</v>
       </c>
       <c r="G301">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H301" t="s">
         <v>78</v>
@@ -25448,7 +25451,7 @@
         <v>77</v>
       </c>
       <c r="G302">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H302" t="s">
         <v>78</v>
@@ -25510,7 +25513,7 @@
         <v>24</v>
       </c>
       <c r="G303">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H303" t="s">
         <v>78</v>
@@ -25572,7 +25575,7 @@
         <v>77</v>
       </c>
       <c r="G304">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H304" t="s">
         <v>78</v>
@@ -25634,7 +25637,7 @@
         <v>77</v>
       </c>
       <c r="G305">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H305" t="s">
         <v>78</v>
@@ -25696,7 +25699,7 @@
         <v>135</v>
       </c>
       <c r="G306">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H306" t="s">
         <v>78</v>
@@ -25758,7 +25761,7 @@
         <v>77</v>
       </c>
       <c r="G307">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H307" t="s">
         <v>78</v>
@@ -25796,7 +25799,7 @@
         <v>135</v>
       </c>
       <c r="G308">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H308" t="s">
         <v>78</v>
@@ -25858,7 +25861,7 @@
         <v>36</v>
       </c>
       <c r="G309">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H309" t="s">
         <v>78</v>
@@ -25920,7 +25923,7 @@
         <v>47</v>
       </c>
       <c r="G310">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H310" t="s">
         <v>78</v>
@@ -25982,7 +25985,7 @@
         <v>135</v>
       </c>
       <c r="G311">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H311" t="s">
         <v>78</v>
@@ -26044,7 +26047,7 @@
         <v>66</v>
       </c>
       <c r="G312">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H312" t="s">
         <v>78</v>
@@ -26085,7 +26088,7 @@
         <v>24</v>
       </c>
       <c r="G313">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H313" t="s">
         <v>78</v>
@@ -26147,7 +26150,7 @@
         <v>47</v>
       </c>
       <c r="G314">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H314" t="s">
         <v>78</v>
@@ -26209,7 +26212,7 @@
         <v>135</v>
       </c>
       <c r="G315">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H315" t="s">
         <v>78</v>
@@ -26271,7 +26274,7 @@
         <v>135</v>
       </c>
       <c r="G316">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H316" t="s">
         <v>78</v>
@@ -26283,7 +26286,7 @@
         <v>229</v>
       </c>
       <c r="K316">
-        <v>17</v>
+        <v>2022</v>
       </c>
       <c r="L316" t="s">
         <v>1804</v>
@@ -26333,7 +26336,7 @@
         <v>47</v>
       </c>
       <c r="G317">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H317" t="s">
         <v>78</v>
@@ -26395,7 +26398,7 @@
         <v>47</v>
       </c>
       <c r="G318">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H318" t="s">
         <v>25</v>
@@ -26451,7 +26454,7 @@
         <v>24</v>
       </c>
       <c r="G319">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H319" t="s">
         <v>78</v>
@@ -26463,7 +26466,7 @@
         <v>80</v>
       </c>
       <c r="K319">
-        <v>13</v>
+        <v>2022</v>
       </c>
       <c r="L319" t="s">
         <v>1816</v>
@@ -26513,7 +26516,7 @@
         <v>66</v>
       </c>
       <c r="G320">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H320" t="s">
         <v>78</v>
@@ -26575,7 +26578,7 @@
         <v>47</v>
       </c>
       <c r="G321">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H321" t="s">
         <v>78</v>
@@ -26637,7 +26640,7 @@
         <v>77</v>
       </c>
       <c r="G322">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H322" t="s">
         <v>78</v>
@@ -26699,7 +26702,7 @@
         <v>47</v>
       </c>
       <c r="G323">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H323" t="s">
         <v>78</v>
@@ -26711,7 +26714,7 @@
         <v>229</v>
       </c>
       <c r="K323">
-        <v>10</v>
+        <v>2022</v>
       </c>
       <c r="L323" t="s">
         <v>460</v>
@@ -26761,7 +26764,7 @@
         <v>36</v>
       </c>
       <c r="G324">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H324" t="s">
         <v>78</v>
@@ -26823,7 +26826,7 @@
         <v>24</v>
       </c>
       <c r="G325">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H325" t="s">
         <v>78</v>
@@ -26885,7 +26888,7 @@
         <v>77</v>
       </c>
       <c r="G326">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H326" t="s">
         <v>78</v>
@@ -26947,7 +26950,7 @@
         <v>135</v>
       </c>
       <c r="G327">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H327" t="s">
         <v>78</v>
@@ -27009,7 +27012,7 @@
         <v>47</v>
       </c>
       <c r="G328">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H328" t="s">
         <v>78</v>
@@ -27071,7 +27074,7 @@
         <v>36</v>
       </c>
       <c r="G329">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H329" t="s">
         <v>78</v>
@@ -27133,7 +27136,7 @@
         <v>24</v>
       </c>
       <c r="G330">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H330" t="s">
         <v>78</v>
@@ -27195,7 +27198,7 @@
         <v>47</v>
       </c>
       <c r="G331">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H331" t="s">
         <v>78</v>
@@ -27257,13 +27260,13 @@
         <v>47</v>
       </c>
       <c r="G332">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H332" t="s">
         <v>25</v>
       </c>
-      <c r="K332" t="s">
-        <v>26</v>
+      <c r="K332">
+        <v>2023</v>
       </c>
       <c r="L332" t="s">
         <v>460</v>
@@ -27313,7 +27316,7 @@
         <v>77</v>
       </c>
       <c r="G333">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H333" t="s">
         <v>78</v>
@@ -27375,7 +27378,7 @@
         <v>66</v>
       </c>
       <c r="G334">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H334" t="s">
         <v>78</v>
@@ -27437,7 +27440,7 @@
         <v>135</v>
       </c>
       <c r="G335">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H335" t="s">
         <v>78</v>
@@ -27499,7 +27502,7 @@
         <v>36</v>
       </c>
       <c r="G336">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H336" t="s">
         <v>78</v>
@@ -27561,7 +27564,7 @@
         <v>66</v>
       </c>
       <c r="G337">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H337" t="s">
         <v>78</v>
@@ -27623,7 +27626,7 @@
         <v>135</v>
       </c>
       <c r="G338">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H338" t="s">
         <v>78</v>
@@ -27685,7 +27688,7 @@
         <v>135</v>
       </c>
       <c r="G339">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H339" t="s">
         <v>78</v>
@@ -27747,7 +27750,7 @@
         <v>135</v>
       </c>
       <c r="G340">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H340" t="s">
         <v>78</v>
@@ -27759,7 +27762,7 @@
         <v>80</v>
       </c>
       <c r="K340">
-        <v>20</v>
+        <v>2022</v>
       </c>
       <c r="L340" t="s">
         <v>1914</v>
@@ -27809,7 +27812,7 @@
         <v>135</v>
       </c>
       <c r="G341">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H341" t="s">
         <v>78</v>
@@ -27871,7 +27874,7 @@
         <v>135</v>
       </c>
       <c r="G342">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H342" t="s">
         <v>78</v>
@@ -27933,7 +27936,7 @@
         <v>57</v>
       </c>
       <c r="G343">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H343" t="s">
         <v>78</v>
@@ -27995,7 +27998,7 @@
         <v>47</v>
       </c>
       <c r="G344">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H344" t="s">
         <v>78</v>
@@ -28057,7 +28060,7 @@
         <v>24</v>
       </c>
       <c r="G345">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H345" t="s">
         <v>78</v>
@@ -28119,7 +28122,7 @@
         <v>36</v>
       </c>
       <c r="G346">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H346" t="s">
         <v>78</v>
@@ -28181,7 +28184,7 @@
         <v>36</v>
       </c>
       <c r="G347">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H347" t="s">
         <v>78</v>
@@ -28243,7 +28246,7 @@
         <v>135</v>
       </c>
       <c r="G348">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H348" t="s">
         <v>78</v>
@@ -28305,7 +28308,7 @@
         <v>24</v>
       </c>
       <c r="G349">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H349" t="s">
         <v>78</v>
@@ -28367,7 +28370,7 @@
         <v>24</v>
       </c>
       <c r="G350">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H350" t="s">
         <v>78</v>
@@ -28429,7 +28432,7 @@
         <v>66</v>
       </c>
       <c r="G351">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H351" t="s">
         <v>78</v>
@@ -28491,7 +28494,7 @@
         <v>24</v>
       </c>
       <c r="G352">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H352" t="s">
         <v>78</v>
@@ -28553,7 +28556,7 @@
         <v>77</v>
       </c>
       <c r="G353">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H353" t="s">
         <v>78</v>
@@ -28615,7 +28618,7 @@
         <v>24</v>
       </c>
       <c r="G354">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H354" t="s">
         <v>78</v>
@@ -28626,8 +28629,8 @@
       <c r="J354" t="s">
         <v>80</v>
       </c>
-      <c r="K354" t="s">
-        <v>26</v>
+      <c r="K354">
+        <v>2023</v>
       </c>
       <c r="L354" t="s">
         <v>1987</v>
@@ -28677,7 +28680,7 @@
         <v>36</v>
       </c>
       <c r="G355">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H355" t="s">
         <v>78</v>
@@ -28739,7 +28742,7 @@
         <v>135</v>
       </c>
       <c r="G356">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H356" t="s">
         <v>78</v>
@@ -28801,7 +28804,7 @@
         <v>36</v>
       </c>
       <c r="G357">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H357" t="s">
         <v>25</v>
@@ -28857,13 +28860,13 @@
         <v>47</v>
       </c>
       <c r="G358">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H358" t="s">
         <v>25</v>
       </c>
       <c r="K358">
-        <v>23</v>
+        <v>2022</v>
       </c>
       <c r="L358" t="s">
         <v>2006</v>
@@ -28913,7 +28916,7 @@
         <v>47</v>
       </c>
       <c r="G359">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H359" t="s">
         <v>25</v>
@@ -28969,7 +28972,7 @@
         <v>24</v>
       </c>
       <c r="G360">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H360" t="s">
         <v>78</v>
@@ -29031,13 +29034,13 @@
         <v>47</v>
       </c>
       <c r="G361">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H361" t="s">
         <v>25</v>
       </c>
-      <c r="K361" t="s">
-        <v>26</v>
+      <c r="K361">
+        <v>2023</v>
       </c>
       <c r="L361" t="s">
         <v>2016</v>
@@ -29087,7 +29090,7 @@
         <v>36</v>
       </c>
       <c r="G362">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H362" t="s">
         <v>78</v>
@@ -29128,7 +29131,7 @@
         <v>47</v>
       </c>
       <c r="G363">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H363" t="s">
         <v>25</v>
@@ -29213,7 +29216,7 @@
         <v>36</v>
       </c>
       <c r="G365">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H365" t="s">
         <v>78</v>
@@ -29275,7 +29278,7 @@
         <v>135</v>
       </c>
       <c r="G366">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H366" t="s">
         <v>78</v>
@@ -29337,7 +29340,7 @@
         <v>36</v>
       </c>
       <c r="G367">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H367" t="s">
         <v>78</v>
@@ -29399,7 +29402,7 @@
         <v>36</v>
       </c>
       <c r="G368">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H368" t="s">
         <v>78</v>
@@ -29461,7 +29464,7 @@
         <v>77</v>
       </c>
       <c r="G369">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H369" t="s">
         <v>78</v>
@@ -29523,7 +29526,7 @@
         <v>36</v>
       </c>
       <c r="G370">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H370" t="s">
         <v>78</v>
@@ -29564,7 +29567,7 @@
         <v>24</v>
       </c>
       <c r="G371">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H371" t="s">
         <v>78</v>
@@ -29626,7 +29629,7 @@
         <v>66</v>
       </c>
       <c r="G372">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H372" t="s">
         <v>25</v>
@@ -29682,7 +29685,7 @@
         <v>77</v>
       </c>
       <c r="G373">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H373" t="s">
         <v>78</v>
@@ -29744,7 +29747,7 @@
         <v>77</v>
       </c>
       <c r="G374">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H374" t="s">
         <v>78</v>
@@ -29806,7 +29809,7 @@
         <v>47</v>
       </c>
       <c r="G375">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H375" t="s">
         <v>78</v>
@@ -29868,7 +29871,7 @@
         <v>77</v>
       </c>
       <c r="G376">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H376" t="s">
         <v>78</v>
@@ -29880,7 +29883,7 @@
         <v>80</v>
       </c>
       <c r="K376">
-        <v>21</v>
+        <v>2022</v>
       </c>
       <c r="L376" t="s">
         <v>2076</v>
@@ -29930,7 +29933,7 @@
         <v>77</v>
       </c>
       <c r="G377">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H377" t="s">
         <v>78</v>
@@ -29992,7 +29995,7 @@
         <v>24</v>
       </c>
       <c r="G378">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H378" t="s">
         <v>78</v>
@@ -30054,7 +30057,7 @@
         <v>66</v>
       </c>
       <c r="G379">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H379" t="s">
         <v>78</v>
@@ -30116,7 +30119,7 @@
         <v>77</v>
       </c>
       <c r="G380">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H380" t="s">
         <v>78</v>
@@ -30178,7 +30181,7 @@
         <v>77</v>
       </c>
       <c r="G381">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H381" t="s">
         <v>78</v>
@@ -30240,7 +30243,7 @@
         <v>66</v>
       </c>
       <c r="G382">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H382" t="s">
         <v>78</v>
@@ -30251,8 +30254,8 @@
       <c r="J382" t="s">
         <v>80</v>
       </c>
-      <c r="K382" t="s">
-        <v>26</v>
+      <c r="K382">
+        <v>2023</v>
       </c>
       <c r="L382" t="s">
         <v>2105</v>
@@ -30302,7 +30305,7 @@
         <v>24</v>
       </c>
       <c r="G383">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H383" t="s">
         <v>78</v>
@@ -30364,7 +30367,7 @@
         <v>66</v>
       </c>
       <c r="G384">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H384" t="s">
         <v>25</v>
@@ -30420,7 +30423,7 @@
         <v>36</v>
       </c>
       <c r="G385">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H385" t="s">
         <v>78</v>
@@ -30482,7 +30485,7 @@
         <v>36</v>
       </c>
       <c r="G386">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H386" t="s">
         <v>78</v>
@@ -30544,7 +30547,7 @@
         <v>24</v>
       </c>
       <c r="G387">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H387" t="s">
         <v>78</v>
@@ -30606,7 +30609,7 @@
         <v>36</v>
       </c>
       <c r="G388">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H388" t="s">
         <v>78</v>
@@ -30668,7 +30671,7 @@
         <v>36</v>
       </c>
       <c r="G389">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H389" t="s">
         <v>78</v>
@@ -30730,7 +30733,7 @@
         <v>24</v>
       </c>
       <c r="G390">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H390" t="s">
         <v>78</v>
@@ -30792,7 +30795,7 @@
         <v>77</v>
       </c>
       <c r="G391">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H391" t="s">
         <v>78</v>
@@ -30803,8 +30806,8 @@
       <c r="J391" t="s">
         <v>80</v>
       </c>
-      <c r="K391" t="s">
-        <v>26</v>
+      <c r="K391">
+        <v>2023</v>
       </c>
       <c r="L391" t="s">
         <v>2149</v>
@@ -30854,7 +30857,7 @@
         <v>24</v>
       </c>
       <c r="G392">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H392" t="s">
         <v>78</v>
@@ -30916,7 +30919,7 @@
         <v>57</v>
       </c>
       <c r="G393">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H393" t="s">
         <v>78</v>
@@ -30978,7 +30981,7 @@
         <v>135</v>
       </c>
       <c r="G394">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H394" t="s">
         <v>78</v>
@@ -31040,7 +31043,7 @@
         <v>66</v>
       </c>
       <c r="G395">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H395" t="s">
         <v>78</v>
@@ -31051,8 +31054,8 @@
       <c r="J395" t="s">
         <v>80</v>
       </c>
-      <c r="K395" t="s">
-        <v>26</v>
+      <c r="K395">
+        <v>2023</v>
       </c>
       <c r="L395" t="s">
         <v>2168</v>
@@ -31102,7 +31105,7 @@
         <v>66</v>
       </c>
       <c r="G396">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H396" t="s">
         <v>78</v>
@@ -31164,7 +31167,7 @@
         <v>135</v>
       </c>
       <c r="G397">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H397" t="s">
         <v>78</v>
@@ -31226,7 +31229,7 @@
         <v>36</v>
       </c>
       <c r="G398">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H398" t="s">
         <v>78</v>
@@ -31288,7 +31291,7 @@
         <v>77</v>
       </c>
       <c r="G399">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H399" t="s">
         <v>78</v>
@@ -31350,7 +31353,7 @@
         <v>24</v>
       </c>
       <c r="G400">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H400" t="s">
         <v>78</v>
@@ -31362,7 +31365,7 @@
         <v>80</v>
       </c>
       <c r="K400">
-        <v>9</v>
+        <v>2022</v>
       </c>
       <c r="L400" t="s">
         <v>2192</v>
@@ -31412,7 +31415,7 @@
         <v>77</v>
       </c>
       <c r="G401">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H401" t="s">
         <v>78</v>
@@ -31474,7 +31477,7 @@
         <v>135</v>
       </c>
       <c r="G402">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H402" t="s">
         <v>78</v>
@@ -31536,7 +31539,7 @@
         <v>66</v>
       </c>
       <c r="G403">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H403" t="s">
         <v>78</v>
@@ -31598,7 +31601,7 @@
         <v>24</v>
       </c>
       <c r="G404">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H404" t="s">
         <v>78</v>
@@ -31609,8 +31612,8 @@
       <c r="J404" t="s">
         <v>80</v>
       </c>
-      <c r="K404" t="s">
-        <v>26</v>
+      <c r="K404">
+        <v>2023</v>
       </c>
       <c r="L404" t="s">
         <v>2213</v>
@@ -31660,7 +31663,7 @@
         <v>77</v>
       </c>
       <c r="G405">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H405" t="s">
         <v>78</v>
@@ -31671,8 +31674,8 @@
       <c r="J405" t="s">
         <v>80</v>
       </c>
-      <c r="K405" t="s">
-        <v>26</v>
+      <c r="K405">
+        <v>2023</v>
       </c>
       <c r="L405" t="s">
         <v>2216</v>
@@ -31722,7 +31725,7 @@
         <v>24</v>
       </c>
       <c r="G406">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H406" t="s">
         <v>78</v>
@@ -31784,7 +31787,7 @@
         <v>77</v>
       </c>
       <c r="G407">
-        <v>1</v>
+        <v>2022</v>
       </c>
       <c r="H407" t="s">
         <v>78</v>

</xml_diff>